<commit_message>
Completion w/ bug fixing but possibly needs more bug fixing
</commit_message>
<xml_diff>
--- a/Snell's Law.xlsx
+++ b/Snell's Law.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitchellyoung/Google Drive/Mitchell's School Work/2017-2018/Sem. 2/Scientific Computing/github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitchellyoung/Google Drive/Mitchell's School Work/2017-2018/Sem. 2/Scientific Computing/github/snell-s-law-myoung2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Inputs</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>If 0≥T≥90</t>
-  </si>
-  <si>
-    <t>If 90&gt;T≥180</t>
   </si>
   <si>
     <t>Slope of first line</t>
@@ -123,20 +120,92 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -145,14 +214,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -204,7 +285,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>0-90, 270-360</a:t>
+              <a:t>Snell's Law Simulation</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -262,61 +343,17 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Calculations!$F$2:$F$3</c:f>
+              <c:f>Calculations!$F$2:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>-1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Calculations!$G$2:$G$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Calculations!$F$3:$F$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -324,15 +361,18 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Calculations!$G$3:$G$4</c:f>
+              <c:f>Calculations!$G$2:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>-1.63245522776191E16</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.63245522776191E16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -347,17 +387,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-936205296"/>
-        <c:axId val="-938711648"/>
+        <c:axId val="-1070704432"/>
+        <c:axId val="-1071365360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-936205296"/>
+        <c:axId val="-1070704432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
           <c:min val="-1.0"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -376,51 +416,18 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-938711648"/>
+        <c:crossAx val="-1071365360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-938711648"/>
+        <c:axId val="-1071365360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
           <c:min val="-1.0"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -436,50 +443,22 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-936205296"/>
+        <c:crossAx val="-1070704432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="bg2"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -518,6 +497,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -634,7 +614,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>-1.63245522776191E16</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -684,7 +664,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>1.63245522776191E16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -699,11 +679,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-934528896"/>
-        <c:axId val="-1183041584"/>
+        <c:axId val="-1073129152"/>
+        <c:axId val="-938297376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-934528896"/>
+        <c:axId val="-1073129152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -761,12 +741,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1183041584"/>
+        <c:crossAx val="-938297376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1183041584"/>
+        <c:axId val="-938297376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -824,7 +804,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-934528896"/>
+        <c:crossAx val="-1073129152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1986,7 +1966,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="'Inputs &amp; Outputs'!$B$2" horiz="1" max="360" page="10" val="270"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="'Inputs &amp; Outputs'!$B$2" horiz="1" max="360" page="10" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2003,8 +1983,8 @@
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>800100</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2028,8 +2008,8 @@
             <a:noFill/>
             <a:ln w="9525">
               <a:miter lim="800000"/>
-              <a:headEnd type="none" w="med" len="med"/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:headEnd/>
+              <a:tailEnd/>
             </a:ln>
           </xdr:spPr>
         </xdr:sp>
@@ -2041,15 +2021,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2074,6 +2054,67 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.03611</cdr:x>
+      <cdr:y>0.56944</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.96389</cdr:x>
+      <cdr:y>0.94444</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Rectangle 1"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="165100" y="1562100"/>
+          <a:ext cx="4241800" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="tx1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2376,7 +2417,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2386,44 +2427,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>270</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
-        <f>Calculations!B6</f>
-        <v>-48.753466631327235</v>
-      </c>
+      <c r="D2" s="12">
+        <f>Calculations!B7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1.33</v>
+      <c r="B5" s="8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2473,7 +2518,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2487,10 +2532,10 @@
       <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1"/>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2498,10 +2543,10 @@
       </c>
       <c r="D2">
         <f>'Inputs &amp; Outputs'!B2</f>
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2">
         <f>C10</f>
@@ -2509,7 +2554,7 @@
       </c>
       <c r="G2">
         <f>IF(OR(D2=90,D2=270),0,IF(D2=180,-D10,D10))</f>
-        <v>0</v>
+        <v>-1.6324552277619072E+16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2530,7 +2575,7 @@
       </c>
       <c r="G4">
         <f>IF(OR(D2=90,D2=270),0,IF(AND(D2&gt;90,D2&lt;270),-D13,D13))</f>
-        <v>0</v>
+        <v>1.6324552277619072E+16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2544,10 +2589,10 @@
       </c>
       <c r="B6">
         <f>ASIN(SIN(D2*PI()/180)*'Inputs &amp; Outputs'!B4/'Inputs &amp; Outputs'!B5)*180/PI()</f>
-        <v>-48.753466631327235</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6">
         <f>C10</f>
@@ -2555,12 +2600,13 @@
       </c>
       <c r="G6">
         <f>D10</f>
-        <v>2.45029690981724E-16</v>
+        <v>-1.6324552277619072E+16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>11</v>
+      <c r="B7">
+        <f>IF(D2&gt;270,B6+360,IF(D2&gt;180,180-B6,IF(D2&gt;90,180-B6,B6)))</f>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -2576,61 +2622,61 @@
       </c>
       <c r="G8">
         <f>-D13</f>
-        <v>-0.87686943155751529</v>
+        <v>-1.6324552277619072E+16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <f>TAN(PI()/180*(D2+90))</f>
-        <v>-2.45029690981724E-16</v>
+        <v>1.6324552277619072E+16</v>
       </c>
       <c r="C10">
         <v>-1</v>
       </c>
       <c r="D10">
         <f>A10*C10</f>
-        <v>2.45029690981724E-16</v>
+        <v>-1.6324552277619072E+16</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <f>TAN(PI()/180*(B6+90))</f>
-        <v>0.87686943155751529</v>
+        <v>1.6324552277619072E+16</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
         <f>A13*C13</f>
-        <v>0.87686943155751529</v>
+        <v>1.6324552277619072E+16</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
+      <c r="A14" s="1"/>
     </row>
     <row r="25" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
     </row>
     <row r="26" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Further bug fix and cosmetic enhancement
</commit_message>
<xml_diff>
--- a/Snell's Law.xlsx
+++ b/Snell's Law.xlsx
@@ -218,22 +218,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -366,13 +366,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-1.63245522776191E16</c:v>
+                  <c:v>0.194380309137719</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.63245522776191E16</c:v>
+                  <c:v>-0.914185755211928</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -387,11 +387,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1070704432"/>
-        <c:axId val="-1071365360"/>
+        <c:axId val="-1183253536"/>
+        <c:axId val="-1010814976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1070704432"/>
+        <c:axId val="-1183253536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -402,12 +402,7 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -416,12 +411,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1071365360"/>
+        <c:crossAx val="-1010814976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1071365360"/>
+        <c:axId val="-1010814976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -432,12 +427,7 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -447,7 +437,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1070704432"/>
+        <c:crossAx val="-1183253536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -614,7 +604,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-1.63245522776191E16</c:v>
+                  <c:v>0.194380309137719</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -664,7 +654,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.63245522776191E16</c:v>
+                  <c:v>-0.914185755211928</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -679,11 +669,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1073129152"/>
-        <c:axId val="-938297376"/>
+        <c:axId val="-1183294224"/>
+        <c:axId val="-1007186032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1073129152"/>
+        <c:axId val="-1183294224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -741,12 +731,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-938297376"/>
+        <c:crossAx val="-1007186032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-938297376"/>
+        <c:axId val="-1007186032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -804,7 +794,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1073129152"/>
+        <c:crossAx val="-1183294224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1966,7 +1956,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="'Inputs &amp; Outputs'!$B$2" horiz="1" max="360" page="10" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="'Inputs &amp; Outputs'!$B$2" horiz="1" max="360" page="10" val="79"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2107,6 +2097,148 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.7</cdr:x>
+      <cdr:y>0.2037</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95556</cdr:x>
+      <cdr:y>0.2963</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3200400" y="558800"/>
+          <a:ext cx="1168400" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Incident</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Medium</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.71389</cdr:x>
+      <cdr:y>0.86111</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.98056</cdr:x>
+      <cdr:y>0.95833</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 3"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3263900" y="2362200"/>
+          <a:ext cx="1219200" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Outgoing </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Medium</a:t>
+          </a:r>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -2417,7 +2549,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2427,48 +2559,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
-        <v>0</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="4">
+        <v>79</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="9">
         <f>Calculations!B7</f>
-        <v>0</v>
+        <v>47.566889913441621</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8">
-        <v>1</v>
+      <c r="B5" s="7">
+        <v>1.33</v>
       </c>
     </row>
   </sheetData>
@@ -2532,10 +2664,10 @@
       <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2543,7 +2675,7 @@
       </c>
       <c r="D2">
         <f>'Inputs &amp; Outputs'!B2</f>
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -2554,7 +2686,7 @@
       </c>
       <c r="G2">
         <f>IF(OR(D2=90,D2=270),0,IF(D2=180,-D10,D10))</f>
-        <v>-1.6324552277619072E+16</v>
+        <v>0.19438030913771864</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2575,7 +2707,7 @@
       </c>
       <c r="G4">
         <f>IF(OR(D2=90,D2=270),0,IF(AND(D2&gt;90,D2&lt;270),-D13,D13))</f>
-        <v>1.6324552277619072E+16</v>
+        <v>-0.91418575521192769</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2589,7 +2721,7 @@
       </c>
       <c r="B6">
         <f>ASIN(SIN(D2*PI()/180)*'Inputs &amp; Outputs'!B4/'Inputs &amp; Outputs'!B5)*180/PI()</f>
-        <v>0</v>
+        <v>47.566889913441621</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
@@ -2600,13 +2732,13 @@
       </c>
       <c r="G6">
         <f>D10</f>
-        <v>-1.6324552277619072E+16</v>
+        <v>0.19438030913771864</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7">
-        <f>IF(D2&gt;270,B6+360,IF(D2&gt;180,180-B6,IF(D2&gt;90,180-B6,B6)))</f>
-        <v>0</v>
+        <f>IF(OR(D2=90,D2=270),D2,IF(D2&gt;270,B6+360,IF(D2&gt;180,180-B6,IF(D2&gt;90,180-B6,B6))))</f>
+        <v>47.566889913441621</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -2622,7 +2754,7 @@
       </c>
       <c r="G8">
         <f>-D13</f>
-        <v>-1.6324552277619072E+16</v>
+        <v>0.91418575521192769</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2636,14 +2768,14 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <f>TAN(PI()/180*(D2+90))</f>
-        <v>1.6324552277619072E+16</v>
+        <v>-0.19438030913771864</v>
       </c>
       <c r="C10">
         <v>-1</v>
       </c>
       <c r="D10">
         <f>A10*C10</f>
-        <v>-1.6324552277619072E+16</v>
+        <v>0.19438030913771864</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -2657,14 +2789,14 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <f>TAN(PI()/180*(B6+90))</f>
-        <v>1.6324552277619072E+16</v>
+        <v>-0.91418575521192769</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
         <f>A13*C13</f>
-        <v>1.6324552277619072E+16</v>
+        <v>-0.91418575521192769</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>